<commit_message>
firmware fixes and improvements
</commit_message>
<xml_diff>
--- a/Avionics/Peripheral Sub Controllers.xlsx
+++ b/Avionics/Peripheral Sub Controllers.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11213"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nyameaama/Documents/A-OneSpace/Converse-Engine/Avionics/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BB19DC2-48A3-DB40-AD66-567A090C8651}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A69314E-4227-254C-8F85-25FD8922E8CD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16280" xr2:uid="{692E348D-7FF9-564E-9138-AA9B07A9E37D}"/>
+    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16280" activeTab="1" xr2:uid="{692E348D-7FF9-564E-9138-AA9B07A9E37D}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Descriptions" sheetId="1" r:id="rId1"/>
+    <sheet name="Base IDs" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="53">
   <si>
     <t>PERIPHERAL SUB CONTROLLERS</t>
   </si>
@@ -124,13 +125,73 @@
   </si>
   <si>
     <t>Description</t>
+  </si>
+  <si>
+    <t>Sensor Peripherals</t>
+  </si>
+  <si>
+    <t>Tag</t>
+  </si>
+  <si>
+    <t>Unique No</t>
+  </si>
+  <si>
+    <t>SBC</t>
+  </si>
+  <si>
+    <t>"01"</t>
+  </si>
+  <si>
+    <t>"02"</t>
+  </si>
+  <si>
+    <t>"03"</t>
+  </si>
+  <si>
+    <t>"04"</t>
+  </si>
+  <si>
+    <t>"05"</t>
+  </si>
+  <si>
+    <t>"06"</t>
+  </si>
+  <si>
+    <t>"07"</t>
+  </si>
+  <si>
+    <t>"08"</t>
+  </si>
+  <si>
+    <t>"09"</t>
+  </si>
+  <si>
+    <t>"10"</t>
+  </si>
+  <si>
+    <t>"11"</t>
+  </si>
+  <si>
+    <t>"12"</t>
+  </si>
+  <si>
+    <t>BaseID</t>
+  </si>
+  <si>
+    <t>Chamber Igniter</t>
+  </si>
+  <si>
+    <t>Igniter Spark Plug</t>
+  </si>
+  <si>
+    <t>"13"</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -149,6 +210,20 @@
     <font>
       <b/>
       <i/>
+      <u/>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Calibri (Body)"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <u/>
       <sz val="16"/>
       <color theme="1"/>
@@ -175,7 +250,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -184,6 +259,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -498,10 +575,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{663FEA1F-6BEA-3042-BEE5-F8E561EDA745}">
-  <dimension ref="A1:F18"/>
+  <dimension ref="A1:F20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -745,10 +822,203 @@
         <v>28</v>
       </c>
     </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B20" t="s">
+        <v>50</v>
+      </c>
+      <c r="D20" t="s">
+        <v>9</v>
+      </c>
+      <c r="E20" t="s">
+        <v>51</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:C1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{254897BC-D891-9C49-ADA5-2EA2A72898BF}">
+  <dimension ref="A1:D18"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="28.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="21" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" t="s">
+        <v>36</v>
+      </c>
+      <c r="C5" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" t="s">
+        <v>36</v>
+      </c>
+      <c r="C6" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" t="s">
+        <v>36</v>
+      </c>
+      <c r="C7" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" t="s">
+        <v>36</v>
+      </c>
+      <c r="C8" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" s="4"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10" t="s">
+        <v>36</v>
+      </c>
+      <c r="C10" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B11" t="s">
+        <v>36</v>
+      </c>
+      <c r="C11" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B12" t="s">
+        <v>36</v>
+      </c>
+      <c r="C12" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B13" t="s">
+        <v>36</v>
+      </c>
+      <c r="C13" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14" s="4"/>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B15" t="s">
+        <v>36</v>
+      </c>
+      <c r="C15" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B16" t="s">
+        <v>36</v>
+      </c>
+      <c r="C16" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>50</v>
+      </c>
+      <c r="B18" t="s">
+        <v>36</v>
+      </c>
+      <c r="C18" t="s">
+        <v>52</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>